<commit_message>
response to reviewers rnd2
</commit_message>
<xml_diff>
--- a/writing/ERL manuscript/2. revise and resubmit/coauthor review/rojas rueda exposures.xlsx
+++ b/writing/ERL manuscript/2. revise and resubmit/coauthor review/rojas rueda exposures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gretam/Documents/Git/lcd2025/writing/ERL manuscript/2. revise and resubmit/coauthor review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A316A73-983D-3248-B1A7-CCD4E1980DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BA0643-3060-7E42-B3F4-46B0AB28F00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28400" windowHeight="15640" xr2:uid="{7CD9AD8A-B386-A340-BFB2-72DD1132B4FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>Author (Year)</t>
   </si>
@@ -427,21 +427,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
     <t>Switzerland- swiss national cohort</t>
   </si>
   <si>
@@ -449,6 +434,39 @@
   </si>
   <si>
     <t>USA- greater Boston area</t>
+  </si>
+  <si>
+    <t>Canada- Ontario</t>
+  </si>
+  <si>
+    <t>Canada- CanCHEC cohort, 30 largest cities in Canada</t>
+  </si>
+  <si>
+    <t>China- CLHLS cohort, 22/31 provinces in China</t>
+  </si>
+  <si>
+    <t>Spain- Barcelona</t>
+  </si>
+  <si>
+    <t>Italy- Rome</t>
+  </si>
+  <si>
+    <t>Australia- Perth, Western Australia</t>
+  </si>
+  <si>
+    <t>climate</t>
+  </si>
+  <si>
+    <t>B, C, D</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -844,26 +862,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74510EB7-C03A-6945-90E0-1D52D4A9D4F7}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="37.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="37.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="18.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="45" style="2" customWidth="1"/>
-    <col min="9" max="9" width="44.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="35.83203125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="3" width="37.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="18.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="45" style="2" customWidth="1"/>
+    <col min="10" max="10" width="44.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="35.83203125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17">
+    <row r="1" spans="1:11" ht="17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -871,305 +889,335 @@
         <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="51">
+    <row r="2" spans="1:11" ht="51">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="68">
+    <row r="3" spans="1:11" ht="68">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="68">
+    <row r="4" spans="1:11" ht="68">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="51">
+    <row r="5" spans="1:11" ht="51">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="51" customHeight="1">
+    <row r="6" spans="1:11" ht="51" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17">
+    <row r="7" spans="1:11" ht="17">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="34">
+    <row r="8" spans="1:11" ht="34">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51">
+    <row r="9" spans="1:11" ht="51">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="68">
+    <row r="10" spans="1:11" ht="68">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="H13" s="4"/>
+    <row r="13" spans="1:11">
+      <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:10">
-      <c r="H14" s="4"/>
+    <row r="14" spans="1:11">
+      <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10">
-      <c r="H15" s="4"/>
+    <row r="15" spans="1:11">
+      <c r="I15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>